<commit_message>
Corrected negative values and deleted sum in Cat_tot
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/extraction/PLIT_S2.xlsx
+++ b/Multi-taxa_data/PLITs/extraction/PLIT_S2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\COMUNE\STUDIO.LAVORO\IMBRSea\Thesis\StatAnalysis\Multi-taxa_data\PLITs\extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238F3150-F18D-4641-9546-3B4B79EB9071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F2CA95-DF8A-4312-8587-F336DCBA8F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2131,10 +2131,10 @@
   <dimension ref="A1:U271"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="K159" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="K165" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A171" sqref="A171"/>
+      <selection pane="bottomRight" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="C48" s="6">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>39</v>
@@ -3112,14 +3112,14 @@
     </row>
     <row r="49" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>883</v>
+        <v>893</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="6">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>37</v>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="C144" s="6">
         <f t="shared" si="2"/>
-        <v>-997</v>
+        <v>3</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>24</v>
@@ -4834,14 +4834,14 @@
     </row>
     <row r="145" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
-        <v>1076</v>
+        <v>2076</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C145" s="6">
         <f t="shared" si="2"/>
-        <v>1004</v>
+        <v>4</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>26</v>
@@ -10086,10 +10086,10 @@
   <dimension ref="A1:U282"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="I138" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="I149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A156" sqref="A156"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10915,7 +10915,7 @@
       </c>
       <c r="C41" s="6">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>29</v>
@@ -10926,14 +10926,14 @@
     </row>
     <row r="42" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>24</v>
@@ -17019,7 +17019,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="J180" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:C198"/>
+      <selection pane="bottomRight" activeCell="A195" sqref="A195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -20659,7 +20659,7 @@
       </c>
       <c r="C196" s="6">
         <f t="shared" si="2"/>
-        <v>-82</v>
+        <v>18</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>29</v>
@@ -20670,7 +20670,7 @@
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" s="14">
-        <v>2816</v>
+        <v>2916</v>
       </c>
       <c r="B197" s="14" t="s">
         <v>38</v>
@@ -20688,7 +20688,7 @@
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" s="14">
-        <v>2820</v>
+        <v>2920</v>
       </c>
       <c r="B198" s="14" t="s">
         <v>10</v>
@@ -20706,7 +20706,7 @@
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" s="14">
-        <v>2823</v>
+        <v>2923</v>
       </c>
       <c r="B199" s="14"/>
       <c r="C199" s="6"/>

</xml_diff>